<commit_message>
add fixes for player names
</commit_message>
<xml_diff>
--- a/data/concordances.xlsx
+++ b/data/concordances.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R\Projects\NBA_fantasy\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{466C13C8-8079-49DE-9914-B1540E375785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84C3C0C7-E24E-45A8-BC57-7A5C3C27C1F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31230" yWindow="1905" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31230" yWindow="1905" windowWidth="21600" windowHeight="11295" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="team_codes" sheetId="1" r:id="rId1"/>
     <sheet name="data_names" sheetId="3" r:id="rId2"/>
     <sheet name="schedule_names" sheetId="4" r:id="rId3"/>
+    <sheet name="player_fix" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="127">
   <si>
     <t>WAS</t>
   </si>
@@ -390,6 +391,24 @@
   </si>
   <si>
     <t>NO</t>
+  </si>
+  <si>
+    <t>player_name</t>
+  </si>
+  <si>
+    <t>new_name</t>
+  </si>
+  <si>
+    <t>Nicolas Claxton</t>
+  </si>
+  <si>
+    <t>Nic Claxton</t>
+  </si>
+  <si>
+    <t>OG Anunoby</t>
+  </si>
+  <si>
+    <t>O.G. Anunoby</t>
   </si>
 </sst>
 </file>
@@ -709,7 +728,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1241,4 +1260,45 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{475F22B5-11CC-4F1F-9A3C-AFFB59C5F189}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>